<commit_message>
Did an alternate. There are advantages, but it is clumsy
</commit_message>
<xml_diff>
--- a/CH-089 Transformation.xlsx
+++ b/CH-089 Transformation.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEDB92C-5E07-4E3D-BA81-840CD292AB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54FD44D-BDE7-4D71-B293-A99177007645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$G$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$G$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$G$7</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -388,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -471,6 +473,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -976,6 +985,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="794" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{09E9E70D-6E91-4BCF-B7CE-C3276C1886D9}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q26"/>
@@ -1505,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A570FC-3CF3-4759-A215-F53E362D4E30}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2389,4 +2425,811 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BFFE9B-6F7C-4A90-B5FD-375080F107DF}">
+  <dimension ref="A1:Q42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="6" width="9.3984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="10" width="9.09765625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="I1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="7">
+        <v>45422</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>45422</v>
+      </c>
+      <c r="C4" s="18">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45421</v>
+      </c>
+      <c r="E4" s="18">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12">
+        <v>45417</v>
+      </c>
+      <c r="G4" s="17">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7">
+        <v>45425</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="24">
+        <v>6</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>45425</v>
+      </c>
+      <c r="C5" s="18">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12">
+        <v>45423</v>
+      </c>
+      <c r="E5" s="18">
+        <v>6</v>
+      </c>
+      <c r="F5" s="12">
+        <v>45418</v>
+      </c>
+      <c r="G5" s="17">
+        <v>6</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7">
+        <v>45427</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="24">
+        <v>17</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>45427</v>
+      </c>
+      <c r="C6" s="18">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12">
+        <v>45425</v>
+      </c>
+      <c r="E6" s="18">
+        <v>15</v>
+      </c>
+      <c r="F6" s="12">
+        <v>45419</v>
+      </c>
+      <c r="G6" s="17">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7">
+        <v>45432</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="24">
+        <v>18</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>45432</v>
+      </c>
+      <c r="C7" s="18">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12">
+        <v>45426</v>
+      </c>
+      <c r="E7" s="18">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12">
+        <v>45423</v>
+      </c>
+      <c r="G7" s="17">
+        <v>6</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7">
+        <v>45437</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="24">
+        <v>13</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>45437</v>
+      </c>
+      <c r="C8" s="18">
+        <v>13</v>
+      </c>
+      <c r="D8" s="13">
+        <v>45427</v>
+      </c>
+      <c r="E8" s="19">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12">
+        <v>45424</v>
+      </c>
+      <c r="G8" s="18">
+        <v>12</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7">
+        <v>45439</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <f>B8+2</f>
+        <v>45439</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="12">
+        <f>F8+1</f>
+        <v>45425</v>
+      </c>
+      <c r="G9" s="18">
+        <v>4</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7">
+        <v>45441</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="24">
+        <v>6</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <f>B9+2</f>
+        <v>45441</v>
+      </c>
+      <c r="C10" s="18">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7">
+        <v>45421</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="24">
+        <v>13</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7">
+        <v>45423</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="24">
+        <v>6</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7">
+        <v>45425</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="24">
+        <v>15</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="7">
+        <v>45426</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="24">
+        <v>13</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+      <c r="I14" s="7">
+        <v>45427</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="9"/>
+      <c r="I15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7">
+        <v>45418</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="7">
+        <v>45419</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="7">
+        <v>45423</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="7">
+        <v>45424</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="11">
+        <v>45425</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="20" t="str" cm="1">
+        <f t="array" ref="B24:D42">_xlfn.LET(
+    _xlpm.d, B2:G10,
+    _xlpm.r, MOD(_xlfn.SEQUENCE(, COLUMNS(_xlpm.d)), 2),
+    _xlpm.e, _xlfn.DROP(_xlpm.d, 2),
+    _xlpm.f, _xlfn._xlws.FILTER(_xlpm.e, _xlpm.r),
+    _xlfn.VSTACK(
+        I2:K2,
+        _xlfn.HSTACK(
+            _xlfn.TOCOL(_xlpm.f, 3, 1),
+            _xlfn.TOCOL(_xlfn.IFS(_xlpm.f, _xlfn.TOROW(_xlfn.TAKE(_xlpm.d, 1), 1)), 3, 1),
+            _xlfn.TOCOL(_xlfn._xlws.FILTER(_xlpm.e, 1 - _xlpm.r), 3, 1)
+        )
+    )
+)</f>
+        <v>Date</v>
+      </c>
+      <c r="C24" s="21" t="str">
+        <v>Product</v>
+      </c>
+      <c r="D24" s="22" t="str">
+        <v>Quantity</v>
+      </c>
+      <c r="F24" s="32" t="str" cm="1">
+        <f t="array" ref="F24:H30">_xlfn.LET(
+_xlpm.d,B2:G10,
+_xlpm.r,MOD(_xlfn.SEQUENCE(,COLUMNS(_xlpm.d)),2),
+_xlpm.e,_xlfn.DROP(_xlpm.d,2),
+_xlpm.f,_xlfn._xlws.FILTER(_xlpm.e,_xlpm.r),
+            _xlfn.IFS(_xlpm.f, _xlfn.TOROW(_xlfn.TAKE(_xlpm.d, 1), 1))
+)</f>
+        <v>A</v>
+      </c>
+      <c r="G24" s="33" t="str">
+        <v>B</v>
+      </c>
+      <c r="H24" s="33" t="str">
+        <v>C</v>
+      </c>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="33"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
+        <v>45422</v>
+      </c>
+      <c r="C25" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D25" s="24">
+        <v>18</v>
+      </c>
+      <c r="F25" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G25" t="str">
+        <v>B</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>45425</v>
+      </c>
+      <c r="C26" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D26" s="24">
+        <v>6</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G26" t="str">
+        <v>B</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
+        <v>45427</v>
+      </c>
+      <c r="C27" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D27" s="24">
+        <v>17</v>
+      </c>
+      <c r="F27" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G27" t="str">
+        <v>B</v>
+      </c>
+      <c r="H27" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
+        <v>45432</v>
+      </c>
+      <c r="C28" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D28" s="24">
+        <v>18</v>
+      </c>
+      <c r="F28" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G28" t="str">
+        <v>B</v>
+      </c>
+      <c r="H28" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
+        <v>45437</v>
+      </c>
+      <c r="C29" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D29" s="24">
+        <v>13</v>
+      </c>
+      <c r="F29" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H29" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
+        <v>45439</v>
+      </c>
+      <c r="C30" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D30" s="24">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="G30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
+        <v>45441</v>
+      </c>
+      <c r="C31" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="D31" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
+        <v>45421</v>
+      </c>
+      <c r="C32" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D32" s="24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="7">
+        <v>45423</v>
+      </c>
+      <c r="C33" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D33" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="7">
+        <v>45425</v>
+      </c>
+      <c r="C34" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D34" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
+        <v>45426</v>
+      </c>
+      <c r="C35" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D35" s="24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="7">
+        <v>45427</v>
+      </c>
+      <c r="C36" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="D36" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
+        <v>45417</v>
+      </c>
+      <c r="C37" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="D37" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
+        <v>45418</v>
+      </c>
+      <c r="C38" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="D38" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="7">
+        <v>45419</v>
+      </c>
+      <c r="C39" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="D39" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="7">
+        <v>45423</v>
+      </c>
+      <c r="C40" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="D40" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="7">
+        <v>45424</v>
+      </c>
+      <c r="C41" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="D41" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>45425</v>
+      </c>
+      <c r="C42" s="25" t="str">
+        <v>C</v>
+      </c>
+      <c r="D42" s="26">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Another alternate. Uses strings. Interesting
</commit_message>
<xml_diff>
--- a/CH-089 Transformation.xlsx
+++ b/CH-089 Transformation.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54FD44D-BDE7-4D71-B293-A99177007645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E680C4-DD6E-495A-9810-73FAECF954E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$G$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$G$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$G$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$G$7</definedName>
   </definedNames>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -89,6 +91,9 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>45422/A/18//45421/B/13//45417/C/15//45425/A/6//45423/B/6//45418/C/6//45427/A/17//45425/B/15//45419/C/12//45432/A/18//45426/B/13//45423/C/6//45437/A/13//45427/B/15//45424/C/12//45439/A/5///B///45425/C/4//45441/A/6///B////C//</t>
   </si>
 </sst>
 </file>
@@ -390,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +486,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2431,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BFFE9B-6F7C-4A90-B5FD-375080F107DF}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3232,4 +3243,860 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B00A07-2BD6-4382-BF4C-909AE2044C3C}">
+  <dimension ref="A1:Q40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="6" width="9.3984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" customWidth="1"/>
+    <col min="8" max="8" width="4.09765625" customWidth="1"/>
+    <col min="9" max="10" width="9.09765625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="I1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="7">
+        <v>45422</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>45422</v>
+      </c>
+      <c r="C4" s="18">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45421</v>
+      </c>
+      <c r="E4" s="18">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12">
+        <v>45417</v>
+      </c>
+      <c r="G4" s="17">
+        <v>15</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7">
+        <v>45425</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="24">
+        <v>6</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>45425</v>
+      </c>
+      <c r="C5" s="18">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12">
+        <v>45423</v>
+      </c>
+      <c r="E5" s="18">
+        <v>6</v>
+      </c>
+      <c r="F5" s="12">
+        <v>45418</v>
+      </c>
+      <c r="G5" s="17">
+        <v>6</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7">
+        <v>45427</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="24">
+        <v>17</v>
+      </c>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>45427</v>
+      </c>
+      <c r="C6" s="18">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12">
+        <v>45425</v>
+      </c>
+      <c r="E6" s="18">
+        <v>15</v>
+      </c>
+      <c r="F6" s="12">
+        <v>45419</v>
+      </c>
+      <c r="G6" s="17">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7">
+        <v>45432</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="24">
+        <v>18</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>45432</v>
+      </c>
+      <c r="C7" s="18">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12">
+        <v>45426</v>
+      </c>
+      <c r="E7" s="18">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12">
+        <v>45423</v>
+      </c>
+      <c r="G7" s="17">
+        <v>6</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7">
+        <v>45437</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="24">
+        <v>13</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>45437</v>
+      </c>
+      <c r="C8" s="18">
+        <v>13</v>
+      </c>
+      <c r="D8" s="13">
+        <v>45427</v>
+      </c>
+      <c r="E8" s="19">
+        <v>15</v>
+      </c>
+      <c r="F8" s="12">
+        <v>45424</v>
+      </c>
+      <c r="G8" s="18">
+        <v>12</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7">
+        <v>45439</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <f>B8+2</f>
+        <v>45439</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="12">
+        <f>F8+1</f>
+        <v>45425</v>
+      </c>
+      <c r="G9" s="18">
+        <v>4</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7">
+        <v>45441</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="24">
+        <v>6</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <f>B9+2</f>
+        <v>45441</v>
+      </c>
+      <c r="C10" s="18">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7">
+        <v>45421</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="24">
+        <v>13</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7">
+        <v>45423</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="24">
+        <v>6</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7">
+        <v>45425</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="24">
+        <v>15</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="7">
+        <v>45426</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="24">
+        <v>13</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+      <c r="I14" s="7">
+        <v>45427</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="9"/>
+      <c r="I15" s="7">
+        <v>45417</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7">
+        <v>45418</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="7">
+        <v>45419</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="7">
+        <v>45423</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="7">
+        <v>45424</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="11">
+        <v>45425</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4" cm="1">
+        <f t="array" ref="B23:D40">_xlfn.LET(
+    _xlpm.a, _xlfn.TEXTSPLIT(
+        SUBSTITUTE(
+            _xlfn.TEXTJOIN("/", , B4:G10 &amp; "/" &amp; B2:G2),
+            "//",
+            "|"
+        ),
+        "/",
+        "|",
+        1
+    ),
+    _xlpm.b, _xlfn._xlws.SORT(_xlfn._xlws.FILTER(_xlpm.a, ISNUMBER(--INDEX(_xlpm.a, , 1))), {2,1}),
+    IFERROR(--_xlpm.b, _xlpm.b)
+)</f>
+        <v>45422</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D23" s="4">
+        <v>18</v>
+      </c>
+      <c r="F23" s="4" t="str" cm="1">
+        <f t="array" ref="F23:K29">B4:G10&amp;"/"&amp;B2:G2</f>
+        <v>45422/A</v>
+      </c>
+      <c r="G23" t="str">
+        <v>18/</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <v>45421/B</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <v>13/</v>
+      </c>
+      <c r="J23" s="5" t="str">
+        <v>45417/C</v>
+      </c>
+      <c r="K23" t="str">
+        <v>15/</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="4">
+        <v>45425</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D24" s="4">
+        <v>6</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <v>45425/A</v>
+      </c>
+      <c r="G24" t="str">
+        <v>6/</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <v>45423/B</v>
+      </c>
+      <c r="I24" s="5" t="str">
+        <v>6/</v>
+      </c>
+      <c r="J24" s="5" t="str">
+        <v>45418/C</v>
+      </c>
+      <c r="K24" t="str">
+        <v>6/</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>45427</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D25" s="4">
+        <v>17</v>
+      </c>
+      <c r="F25" s="4" t="str">
+        <v>45427/A</v>
+      </c>
+      <c r="G25" t="str">
+        <v>17/</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <v>45425/B</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <v>15/</v>
+      </c>
+      <c r="J25" s="5" t="str">
+        <v>45419/C</v>
+      </c>
+      <c r="K25" t="str">
+        <v>12/</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>45432</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D26" s="4">
+        <v>18</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <v>45432/A</v>
+      </c>
+      <c r="G26" t="str">
+        <v>18/</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <v>45426/B</v>
+      </c>
+      <c r="I26" s="5" t="str">
+        <v>13/</v>
+      </c>
+      <c r="J26" s="5" t="str">
+        <v>45423/C</v>
+      </c>
+      <c r="K26" t="str">
+        <v>6/</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>45437</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D27" s="4">
+        <v>13</v>
+      </c>
+      <c r="F27" s="4" t="str">
+        <v>45437/A</v>
+      </c>
+      <c r="G27" t="str">
+        <v>13/</v>
+      </c>
+      <c r="H27" t="str">
+        <v>45427/B</v>
+      </c>
+      <c r="I27" s="5" t="str">
+        <v>15/</v>
+      </c>
+      <c r="J27" s="5" t="str">
+        <v>45424/C</v>
+      </c>
+      <c r="K27" t="str">
+        <v>12/</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>45439</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="F28" s="4" t="str">
+        <v>45439/A</v>
+      </c>
+      <c r="G28" t="str">
+        <v>5/</v>
+      </c>
+      <c r="H28" t="str">
+        <v>/B</v>
+      </c>
+      <c r="I28" s="5" t="str">
+        <v>/</v>
+      </c>
+      <c r="J28" s="5" t="str">
+        <v>45425/C</v>
+      </c>
+      <c r="K28" t="str">
+        <v>4/</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>45441</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="D29" s="4">
+        <v>6</v>
+      </c>
+      <c r="F29" s="4" t="str">
+        <v>45441/A</v>
+      </c>
+      <c r="G29" t="str">
+        <v>6/</v>
+      </c>
+      <c r="H29" t="str">
+        <v>/B</v>
+      </c>
+      <c r="I29" s="5" t="str">
+        <v>/</v>
+      </c>
+      <c r="J29" s="5" t="str">
+        <v>/C</v>
+      </c>
+      <c r="K29" t="str">
+        <v>/</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>45421</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D30" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>45423</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6</v>
+      </c>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>45425</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D32" s="4">
+        <v>15</v>
+      </c>
+      <c r="E32" s="36"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>45426</v>
+      </c>
+      <c r="C33" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D33" s="4">
+        <v>13</v>
+      </c>
+      <c r="F33" s="35" t="str" cm="1">
+        <f t="array" ref="F33">_xlfn.TEXTJOIN("/", , B4:G10 &amp; "/" &amp; B2:G2)</f>
+        <v>45422/A/18//45421/B/13//45417/C/15//45425/A/6//45423/B/6//45418/C/6//45427/A/17//45425/B/15//45419/C/12//45432/A/18//45426/B/13//45423/C/6//45437/A/13//45427/B/15//45424/C/12//45439/A/5///B///45425/C/4//45441/A/6///B////C//</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>45427</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="D34" s="4">
+        <v>15</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>45417</v>
+      </c>
+      <c r="C35" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D35" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>45418</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D36" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>45419</v>
+      </c>
+      <c r="C37" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D37" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>45423</v>
+      </c>
+      <c r="C38" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D38" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>45424</v>
+      </c>
+      <c r="C39" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D39" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>45425</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="D40" s="4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>